<commit_message>
CLEANING AND REDOING MESSED UP SCRAPS
</commit_message>
<xml_diff>
--- a/COGA_GenFundRevenue_Mar.xlsx
+++ b/COGA_GenFundRevenue_Mar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Interns-Fellowships\Alexis 2020\GDP Project\GDP Data Vis\IL-Budget-Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13130E03-1B86-4F59-9E76-26DA70206FDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C51A26-861F-4A8B-927D-F90988E588A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,38 +20,150 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>UPDATED CGFA [Mar-19] vs. ENACTED BUDGET [June-18]</t>
-  </si>
-  <si>
-    <t>FY 2019 GENERAL FUNDS REVENUE ESTIMATE</t>
-  </si>
-  <si>
-    <t>FY FY 2019 FY 2019</t>
-  </si>
-  <si>
-    <t>Revenue Sources</t>
-  </si>
-  <si>
-    <t>FY 2019 CGFA MAR-19</t>
-  </si>
-  <si>
-    <t>FY 2019 FINAL BUDGET  JUNE-19</t>
-  </si>
-  <si>
-    <t>$ DIFFERENCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State taxes </t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
+  <si>
+    <t>FY 2020 and UPDATED FY 2019 GENERAL FUNDS REVENUE CGFA ESTIMATES [per Current Law]</t>
+  </si>
+  <si>
+    <t>(millions)</t>
+  </si>
+  <si>
+    <t>REVENUE SOURCES</t>
+  </si>
+  <si>
+    <t>DIFFERENCES</t>
+  </si>
+  <si>
+    <t>Personal Income Tax</t>
+  </si>
+  <si>
+    <t>Corporate Income Tax (regular)</t>
+  </si>
+  <si>
+    <t>Sales Taxes</t>
+  </si>
+  <si>
+    <t>Public Utility (regular)</t>
+  </si>
+  <si>
+    <t>Cigarette Tax</t>
+  </si>
+  <si>
+    <t>Liquor Gallonage Taxes</t>
+  </si>
+  <si>
+    <t>Vehicle Use Tax</t>
+  </si>
+  <si>
+    <t>Inheritance Tax</t>
+  </si>
+  <si>
+    <t>Insurance Taxes &amp; Fees</t>
+  </si>
+  <si>
+    <t>Corporate Franchise Tax &amp; Fees</t>
+  </si>
+  <si>
+    <t>Interest on State Funds &amp; Investments</t>
+  </si>
+  <si>
+    <t>Cook County Intergovernmental Transfer</t>
+  </si>
+  <si>
+    <t>Other Sources</t>
+  </si>
+  <si>
+    <t>Subtotal</t>
+  </si>
+  <si>
+    <t>Transfers</t>
+  </si>
+  <si>
+    <t>Lottery</t>
+  </si>
+  <si>
+    <t>Riverboat transfers and receipts</t>
+  </si>
+  <si>
+    <t>Proceeds from sale of 10th license</t>
+  </si>
+  <si>
+    <t>Refund Fund</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Total State Sources</t>
+  </si>
+  <si>
+    <t>Federal Sources [Base]</t>
+  </si>
+  <si>
+    <t>Subtotal Federal &amp; State Sources</t>
+  </si>
+  <si>
+    <t>Nongeneral Funds Distribution:</t>
+  </si>
+  <si>
+    <t>Personal Income Tax [9.7% '19]</t>
+  </si>
+  <si>
+    <t>Corporate Income Tax [15.5% '19]</t>
+  </si>
+  <si>
+    <t>Local Government Distributive Fund</t>
+  </si>
+  <si>
+    <t>Corporate Income Tax</t>
+  </si>
+  <si>
+    <t>Sales Tax Distribution to the PTF and DPTF</t>
+  </si>
+  <si>
+    <t>Subtotal General Funds</t>
+  </si>
+  <si>
+    <t>Interfund Borrowing</t>
+  </si>
+  <si>
+    <t>Treasurer's Investment Borrowing</t>
+  </si>
+  <si>
+    <t>Total Revenues General Funds</t>
+  </si>
+  <si>
+    <t>FY 2019 CGFA  MAR-19</t>
+  </si>
+  <si>
+    <t>FY 2019 FINAL BUDGET JUNE -18</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -79,8 +191,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -377,49 +504,515 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:F6"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B25" sqref="B1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="7" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="7">
+        <v>21588</v>
+      </c>
+      <c r="C4" s="7">
+        <v>21263</v>
+      </c>
+      <c r="D4" s="7">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="7">
+        <v>2834</v>
+      </c>
+      <c r="C5" s="7">
+        <v>2618</v>
+      </c>
+      <c r="D5" s="7">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="7">
+        <v>8775</v>
+      </c>
+      <c r="C6" s="7">
+        <v>8679</v>
+      </c>
+      <c r="D6" s="7">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="7">
+        <v>879</v>
+      </c>
+      <c r="C7" s="7">
+        <v>878</v>
+      </c>
+      <c r="D7" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="7">
+        <v>348</v>
+      </c>
+      <c r="C8" s="7">
+        <v>353</v>
+      </c>
+      <c r="D8" s="7">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="7">
+        <v>174</v>
+      </c>
+      <c r="C9" s="7">
+        <v>174</v>
+      </c>
+      <c r="D9" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="7">
+        <v>31</v>
+      </c>
+      <c r="C10" s="7">
+        <v>30</v>
+      </c>
+      <c r="D10" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="7">
+        <v>350</v>
+      </c>
+      <c r="C11" s="7">
+        <v>290</v>
+      </c>
+      <c r="D11" s="7">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="7">
+        <v>421</v>
+      </c>
+      <c r="C12" s="7">
+        <v>405</v>
+      </c>
+      <c r="D12" s="7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="7">
+        <v>205</v>
+      </c>
+      <c r="C13" s="7">
+        <v>205</v>
+      </c>
+      <c r="D13" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="7">
+        <v>125</v>
+      </c>
+      <c r="C14" s="7">
+        <v>112</v>
+      </c>
+      <c r="D14" s="7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="7">
+        <v>244</v>
+      </c>
+      <c r="C15" s="7">
+        <v>244</v>
+      </c>
+      <c r="D15" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="7">
+        <v>676</v>
+      </c>
+      <c r="C16" s="7">
+        <v>1004</v>
+      </c>
+      <c r="D16" s="7">
+        <v>-328</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="7">
+        <v>36650</v>
+      </c>
+      <c r="C17" s="7">
+        <v>36255</v>
+      </c>
+      <c r="D17" s="7">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="7">
+        <v>731</v>
+      </c>
+      <c r="C19" s="7">
+        <v>733</v>
+      </c>
+      <c r="D19" s="7">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="7">
+        <v>261</v>
+      </c>
+      <c r="C20" s="7">
+        <v>266</v>
+      </c>
+      <c r="D20" s="7">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="7">
+        <v>10</v>
+      </c>
+      <c r="C21" s="7">
+        <v>10</v>
+      </c>
+      <c r="D21" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="7">
+        <v>327</v>
+      </c>
+      <c r="C22" s="7">
+        <v>200</v>
+      </c>
+      <c r="D22" s="7">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="7">
+        <v>676</v>
+      </c>
+      <c r="C23" s="7">
+        <v>687</v>
+      </c>
+      <c r="D23" s="7">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="7">
+        <v>38655</v>
+      </c>
+      <c r="C24" s="7">
+        <v>38151</v>
+      </c>
+      <c r="D24" s="7">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="7">
+        <v>3050</v>
+      </c>
+      <c r="C25" s="7">
+        <v>3785</v>
+      </c>
+      <c r="D25" s="7">
+        <v>-735</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="7">
+        <v>41705</v>
+      </c>
+      <c r="C26" s="7">
+        <v>41936</v>
+      </c>
+      <c r="D26" s="7">
+        <v>-231</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="7">
+        <v>-2094</v>
+      </c>
+      <c r="C29" s="7">
+        <v>-2063</v>
+      </c>
+      <c r="D29" s="7">
+        <v>-31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="7">
+        <v>-439</v>
+      </c>
+      <c r="C30" s="7">
+        <v>-406</v>
+      </c>
+      <c r="D30" s="7">
+        <v>-33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>4</v>
       </c>
-      <c r="E5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
+      <c r="B32" s="7">
+        <v>-1122</v>
+      </c>
+      <c r="C32" s="7">
+        <v>-1105</v>
+      </c>
+      <c r="D32" s="7">
+        <v>-17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="7">
+        <v>-156</v>
+      </c>
+      <c r="C33" s="7">
+        <v>-146</v>
+      </c>
+      <c r="D33" s="7">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" s="7">
+        <v>-508</v>
+      </c>
+      <c r="C34" s="7">
+        <v>-496</v>
+      </c>
+      <c r="D34" s="7">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" s="7">
+        <v>37386</v>
+      </c>
+      <c r="C35" s="7">
+        <v>37720</v>
+      </c>
+      <c r="D35" s="7">
+        <v>-334</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" s="7">
+        <v>250</v>
+      </c>
+      <c r="C36" s="7">
+        <v>800</v>
+      </c>
+      <c r="D36" s="7">
+        <v>-550</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" s="7">
+        <v>700</v>
+      </c>
+      <c r="C37" s="7">
+        <v>0</v>
+      </c>
+      <c r="D37" s="7">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="7">
+        <v>38336</v>
+      </c>
+      <c r="C38" s="7">
+        <v>38520</v>
+      </c>
+      <c r="D38" s="7">
+        <v>-184</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>